<commit_message>
add support for spreadsheet extension ^1.1
</commit_message>
<xml_diff>
--- a/Tests/Fixtures/01_fixture.xlsx
+++ b/Tests/Fixtures/01_fixture.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thorsten.hogenkamp\Documents\Projekte\DUERR\duerr-internet\web\typo3conf\ext\udg_spreadsheets\Tests\Fixtures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Thorsten\Documents\Projekte\typo3-extensions\spreadsheets\Tests\Fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Fixture1" sheetId="2" r:id="rId1"/>
     <sheet name="Fixture2" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>x</t>
   </si>
@@ -78,11 +78,59 @@
       <t>Tief</t>
     </r>
   </si>
+  <si>
+    <t>Summe</t>
+  </si>
+  <si>
+    <t>Multiplikat</t>
+  </si>
+  <si>
+    <t>Division</t>
+  </si>
+  <si>
+    <t>Subtraktion</t>
+  </si>
+  <si>
+    <t>formatted</t>
+  </si>
+  <si>
+    <t>Wissenschaftlich</t>
+  </si>
+  <si>
+    <t>Zahl - Tausenderzeichen - 3 Stellen</t>
+  </si>
+  <si>
+    <t>Währung - japanisch - 3 Stellen</t>
+  </si>
+  <si>
+    <t>Währung - russisch - 1 Stelle</t>
+  </si>
+  <si>
+    <t>Prozent - 2 Stellen</t>
+  </si>
+  <si>
+    <t>Währung - Euro - 1 Stelle</t>
+  </si>
+  <si>
+    <t>Datum</t>
+  </si>
+  <si>
+    <t>Wissenschaftlich #2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="7">
+    <numFmt numFmtId="164" formatCode="#,##0.0\ &quot;€&quot;"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
+    <numFmt numFmtId="166" formatCode="[$¥-411]#,##0.000"/>
+    <numFmt numFmtId="167" formatCode="#,##0.0\ [$₽-419]"/>
+    <numFmt numFmtId="168" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="169" formatCode="0.0E+00"/>
+    <numFmt numFmtId="171" formatCode="0.000E+00"/>
+  </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -274,7 +322,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -300,6 +348,13 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -309,6 +364,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
@@ -631,10 +690,10 @@
       <c r="C2" s="3">
         <v>70</v>
       </c>
-      <c r="D2" s="19">
+      <c r="D2" s="26">
         <v>80</v>
       </c>
-      <c r="E2" s="19"/>
+      <c r="E2" s="26"/>
       <c r="F2" s="5" t="s">
         <v>0</v>
       </c>
@@ -673,7 +732,7 @@
       <c r="A6" s="7">
         <v>2014</v>
       </c>
-      <c r="B6" s="20">
+      <c r="B6" s="27">
         <v>2015</v>
       </c>
       <c r="C6" s="8">
@@ -693,7 +752,7 @@
       <c r="A7" s="10">
         <v>50</v>
       </c>
-      <c r="B7" s="21"/>
+      <c r="B7" s="28"/>
       <c r="C7" s="11">
         <v>70</v>
       </c>
@@ -722,12 +781,132 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>123</v>
+      </c>
+      <c r="B1">
+        <v>456</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="29"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <f>A1+B1</f>
+        <v>579</v>
+      </c>
+      <c r="C2" s="25">
+        <f>B2</f>
+        <v>579</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <f>A1-B1</f>
+        <v>-333</v>
+      </c>
+      <c r="C3" s="19">
+        <f>B3</f>
+        <v>-333</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <f>A1*B1</f>
+        <v>56088</v>
+      </c>
+      <c r="C4" s="20">
+        <f>B4</f>
+        <v>56088</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <f>B1/A1</f>
+        <v>3.7073170731707319</v>
+      </c>
+      <c r="C5" s="21">
+        <f>B5</f>
+        <v>3.7073170731707319</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="22">
+        <f>B5</f>
+        <v>3.7073170731707319</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="23">
+        <f>B5</f>
+        <v>3.7073170731707319</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="24">
+        <v>43544</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="30">
+        <f>B2</f>
+        <v>579</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>